<commit_message>
Create merchant All Scenarios Covered
</commit_message>
<xml_diff>
--- a/Testdata/TestCaseData.xlsx
+++ b/Testdata/TestCaseData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Raman\TestNG_Framework\Signature_Automation_Framework\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486DE0F9-17DE-4CA9-A598-8512566B369B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C0A1BA-0E0E-4C7A-90C1-8B3CDB3E3A22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="429">
   <si>
     <t>Runmode</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Amal Delgado</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Airports, Airport Terminals</t>
   </si>
   <si>
@@ -133,18 +130,6 @@
   </si>
   <si>
     <t>Airlines and Ticketing Services</t>
-  </si>
-  <si>
-    <t>QR Code</t>
-  </si>
-  <si>
-    <t>gonyvivec@mailinator.com</t>
-  </si>
-  <si>
-    <t>Dolorem@facebook.com</t>
-  </si>
-  <si>
-    <t>Unde@twitter.com</t>
   </si>
   <si>
     <t>JPG File
@@ -229,13 +214,7 @@
     <t>Trading_Branding_Name</t>
   </si>
   <si>
-    <t>Same_as_Legal_Name</t>
-  </si>
-  <si>
     <t>Name_of_Store_Shop</t>
-  </si>
-  <si>
-    <t>Merchant_Type</t>
   </si>
   <si>
     <t>Legal_License</t>
@@ -1056,9 +1035,6 @@
     <t>Legal_Name_of_Business</t>
   </si>
   <si>
-    <t>Add_Notes</t>
-  </si>
-  <si>
     <t>218</t>
   </si>
   <si>
@@ -1209,9 +1185,6 @@
     <t>CMP_Merchant_Category</t>
   </si>
   <si>
-    <t>CMP_Reference_Number_QR_Code</t>
-  </si>
-  <si>
     <t>ramankumar</t>
   </si>
   <si>
@@ -1296,9 +1269,6 @@
     <t>Test007</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>Raman</t>
   </si>
   <si>
@@ -1306,14 +1276,61 @@
   </si>
   <si>
     <t>Kumar</t>
+  </si>
+  <si>
+    <t>CMP_Add_Notes</t>
+  </si>
+  <si>
+    <t>CMP_Merchant_Type</t>
+  </si>
+  <si>
+    <t>CMP_Branch</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Blocked</t>
+  </si>
+  <si>
+    <t>Expired</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>CMP_BrandingNameSameAsLegalName</t>
+  </si>
+  <si>
+    <t>CMP_StoreNameSameAsLegalName</t>
+  </si>
+  <si>
+    <t>LegalNameCheckBox</t>
+  </si>
+  <si>
+    <t>CMP_Reference_Number</t>
+  </si>
+  <si>
+    <t>Business to Business</t>
+  </si>
+  <si>
+    <t>test@qatest.com</t>
+  </si>
+  <si>
+    <t>test@facebook.com</t>
+  </si>
+  <si>
+    <t>test@twitter.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1949,92 +1966,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CC3"/>
+  <dimension ref="A1:CC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="AN3" sqref="AN3"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="6.61328125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="18.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="25.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="12.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="12" width="25.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="12" width="24.42578125" collapsed="true"/>
-    <col min="10" max="12" bestFit="true" customWidth="true" style="12" width="20.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="12" width="7.42578125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="12" width="23.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="12" width="20.42578125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="12" width="12.42578125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="12" width="20.140625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="12" width="15.7109375" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="12" width="19.85546875" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="12" width="26.7109375" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="12" width="24.140625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="12" width="33.0" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="12" width="26.42578125" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="2" width="29.0" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="2" width="27.7109375" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="2" width="30.5703125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="2" width="26.0" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="2" width="23.7109375" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="2" width="26.7109375" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="2" width="26.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="2" width="25.7109375" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="2" width="22.42578125" collapsed="true"/>
-    <col min="34" max="34" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
-    <col min="35" max="35" customWidth="true" style="2" width="21.0" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" style="2" width="19.7109375" collapsed="true"/>
-    <col min="37" max="37" customWidth="true" style="2" width="22.42578125" collapsed="true"/>
-    <col min="38" max="38" customWidth="true" style="2" width="15.85546875" collapsed="true"/>
-    <col min="39" max="39" customWidth="true" style="2" width="33.140625" collapsed="true"/>
-    <col min="40" max="40" customWidth="true" style="2" width="16.7109375" collapsed="true"/>
-    <col min="41" max="41" customWidth="true" style="2" width="19.28515625" collapsed="true"/>
-    <col min="42" max="42" customWidth="true" style="2" width="17.28515625" collapsed="true"/>
-    <col min="43" max="43" customWidth="true" style="2" width="26.28515625" collapsed="true"/>
-    <col min="44" max="44" customWidth="true" style="2" width="26.42578125" collapsed="true"/>
-    <col min="45" max="45" customWidth="true" style="2" width="29.85546875" collapsed="true"/>
-    <col min="46" max="46" customWidth="true" style="12" width="21.5703125" collapsed="true"/>
-    <col min="47" max="47" customWidth="true" style="12" width="16.7109375" collapsed="true"/>
-    <col min="48" max="48" customWidth="true" style="12" width="18.42578125" collapsed="true"/>
-    <col min="49" max="49" customWidth="true" style="12" width="18.7109375" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" style="12" width="21.85546875" collapsed="true"/>
-    <col min="51" max="51" customWidth="true" style="12" width="11.5703125" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" style="12" width="19.7109375" collapsed="true"/>
-    <col min="53" max="53" customWidth="true" style="12" width="23.140625" collapsed="true"/>
-    <col min="54" max="54" customWidth="true" style="12" width="19.140625" collapsed="true"/>
-    <col min="55" max="55" customWidth="true" style="12" width="20.140625" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" style="12" width="16.42578125" collapsed="true"/>
-    <col min="57" max="57" customWidth="true" style="12" width="18.5703125" collapsed="true"/>
-    <col min="58" max="58" customWidth="true" style="12" width="21.85546875" collapsed="true"/>
-    <col min="59" max="59" customWidth="true" style="12" width="22.28515625" collapsed="true"/>
-    <col min="60" max="60" customWidth="true" style="12" width="27.42578125" collapsed="true"/>
-    <col min="61" max="61" customWidth="true" style="12" width="36.28515625" collapsed="true"/>
-    <col min="62" max="62" customWidth="true" style="12" width="12.5703125" collapsed="true"/>
-    <col min="63" max="63" customWidth="true" style="12" width="17.28515625" collapsed="true"/>
-    <col min="64" max="64" customWidth="true" style="12" width="20.42578125" collapsed="true"/>
-    <col min="65" max="65" customWidth="true" style="12" width="22.0" collapsed="true"/>
-    <col min="66" max="66" customWidth="true" style="12" width="29.28515625" collapsed="true"/>
-    <col min="67" max="67" customWidth="true" style="12" width="23.42578125" collapsed="true"/>
-    <col min="68" max="70" bestFit="true" customWidth="true" style="12" width="19.28515625" collapsed="true"/>
-    <col min="71" max="71" customWidth="true" style="12" width="17.28515625" collapsed="true"/>
-    <col min="72" max="72" bestFit="true" customWidth="true" style="12" width="16.7109375" collapsed="true"/>
-    <col min="73" max="73" bestFit="true" customWidth="true" style="12" width="20.28515625" collapsed="true"/>
-    <col min="74" max="74" bestFit="true" customWidth="true" style="12" width="14.42578125" collapsed="true"/>
-    <col min="75" max="75" bestFit="true" customWidth="true" style="12" width="22.0" collapsed="true"/>
-    <col min="76" max="76" bestFit="true" customWidth="true" style="12" width="20.7109375" collapsed="true"/>
-    <col min="77" max="77" customWidth="true" style="12" width="23.0" collapsed="true"/>
-    <col min="78" max="78" customWidth="true" style="12" width="23.7109375" collapsed="true"/>
-    <col min="79" max="79" bestFit="true" customWidth="true" style="12" width="19.7109375" collapsed="true"/>
-    <col min="80" max="80" customWidth="true" style="12" width="19.28515625" collapsed="true"/>
-    <col min="81" max="81" customWidth="true" style="12" width="32.0" collapsed="true"/>
-    <col min="82" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="25" style="12" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.42578125" style="12" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="38.140625" style="12" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.85546875" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="33.28515625" style="12" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.85546875" style="12" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="35.7109375" style="12" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.42578125" style="12" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.42578125" style="12" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="20.140625" style="12" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.7109375" style="12" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="19.85546875" style="12" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="26.7109375" style="12" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="24.140625" style="12" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="23.85546875" style="12" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="26.42578125" style="12" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="29" style="2" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="27.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="30.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="21.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="23.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="26.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="23.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="26.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="25.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="22.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="18.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="21" style="2" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="19.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="22.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="15.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="33.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="16.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="17.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="26.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="26.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="29.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="21.5703125" style="12" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="16.7109375" style="12" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="18.42578125" style="12" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="18.7109375" style="12" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="21.85546875" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="11.5703125" style="12" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="19.7109375" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="23.140625" style="12" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="19.140625" style="12" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="20.140625" style="12" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="16.42578125" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="18.5703125" style="12" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="21.85546875" style="12" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="22.28515625" style="12" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="27.42578125" style="12" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="20.28515625" style="12" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="12.5703125" style="12" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="17.28515625" style="12" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="20.42578125" style="12" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="22" style="12" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="29.28515625" style="12" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="23.42578125" style="12" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="33.85546875" style="12" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="41.140625" style="12" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="21" style="12" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="26.7109375" style="12" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="25.85546875" style="12" customWidth="1" collapsed="1"/>
+    <col min="73" max="73" width="23.42578125" style="12" customWidth="1" collapsed="1"/>
+    <col min="74" max="74" width="23.5703125" style="12" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="27" style="12" customWidth="1" collapsed="1"/>
+    <col min="76" max="76" width="29" style="12" customWidth="1" collapsed="1"/>
+    <col min="77" max="77" width="23" style="12" customWidth="1" collapsed="1"/>
+    <col min="78" max="78" width="24.140625" style="12" customWidth="1" collapsed="1"/>
+    <col min="79" max="79" width="20.140625" style="12" customWidth="1" collapsed="1"/>
+    <col min="80" max="80" width="19.28515625" style="12" customWidth="1" collapsed="1"/>
+    <col min="81" max="81" width="32" style="12" customWidth="1" collapsed="1"/>
+    <col min="82" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2122,7 +2143,7 @@
       <c r="CB1" s="21"/>
       <c r="CC1" s="21"/>
     </row>
-    <row r="2" spans="1:81" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:81" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
@@ -2145,235 +2166,233 @@
         <v>16</v>
       </c>
       <c r="H2" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="M2" s="24" t="s">
+        <v>415</v>
+      </c>
+      <c r="N2" s="24" t="s">
+        <v>414</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>413</v>
+      </c>
+      <c r="P2" s="24" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q2" s="24" t="s">
+        <v>377</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>378</v>
+      </c>
+      <c r="S2" s="24" t="s">
+        <v>379</v>
+      </c>
+      <c r="T2" s="24" t="s">
+        <v>380</v>
+      </c>
+      <c r="U2" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="V2" s="24" t="s">
+        <v>424</v>
+      </c>
+      <c r="W2" s="24" t="s">
+        <v>336</v>
+      </c>
+      <c r="X2" s="24" t="s">
+        <v>337</v>
+      </c>
+      <c r="Y2" s="24" t="s">
         <v>338</v>
       </c>
-      <c r="I2" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="J2" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="K2" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="L2" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="M2" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="O2" s="24" t="s">
+      <c r="Z2" s="24" t="s">
         <v>339</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="AA2" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="AB2" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="AC2" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="AD2" s="24" t="s">
+        <v>342</v>
+      </c>
+      <c r="AE2" s="24" t="s">
+        <v>341</v>
+      </c>
+      <c r="AF2" s="24" t="s">
+        <v>356</v>
+      </c>
+      <c r="AG2" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="AH2" s="24" t="s">
+        <v>358</v>
+      </c>
+      <c r="AI2" s="24" t="s">
+        <v>359</v>
+      </c>
+      <c r="AJ2" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="AK2" s="24" t="s">
+        <v>361</v>
+      </c>
+      <c r="AL2" s="24" t="s">
+        <v>362</v>
+      </c>
+      <c r="AM2" s="24" t="s">
+        <v>363</v>
+      </c>
+      <c r="AN2" s="24" t="s">
+        <v>364</v>
+      </c>
+      <c r="AO2" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="AP2" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="AQ2" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="AR2" s="24" t="s">
+        <v>347</v>
+      </c>
+      <c r="AS2" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="AT2" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="AU2" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="AV2" s="24" t="s">
+        <v>370</v>
+      </c>
+      <c r="AW2" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="AX2" s="24" t="s">
+        <v>371</v>
+      </c>
+      <c r="AY2" s="24" t="s">
+        <v>372</v>
+      </c>
+      <c r="AZ2" s="24" t="s">
+        <v>373</v>
+      </c>
+      <c r="BA2" s="24" t="s">
+        <v>374</v>
+      </c>
+      <c r="BB2" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="BC2" s="24" t="s">
+        <v>350</v>
+      </c>
+      <c r="BD2" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="BE2" s="24" t="s">
+        <v>351</v>
+      </c>
+      <c r="BF2" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="BG2" s="24" t="s">
         <v>384</v>
       </c>
-      <c r="Q2" s="24" t="s">
-        <v>385</v>
-      </c>
-      <c r="R2" s="24" t="s">
-        <v>386</v>
-      </c>
-      <c r="S2" s="24" t="s">
+      <c r="BH2" s="24" t="s">
         <v>387</v>
       </c>
-      <c r="T2" s="24" t="s">
+      <c r="BI2" s="24" t="s">
         <v>388</v>
       </c>
-      <c r="U2" s="24" t="s">
+      <c r="BJ2" s="24" t="s">
         <v>389</v>
       </c>
-      <c r="V2" s="24" t="s">
+      <c r="BK2" s="24" t="s">
+        <v>406</v>
+      </c>
+      <c r="BL2" s="24" t="s">
+        <v>407</v>
+      </c>
+      <c r="BM2" s="24" t="s">
         <v>390</v>
       </c>
-      <c r="W2" s="24" t="s">
-        <v>344</v>
-      </c>
-      <c r="X2" s="24" t="s">
-        <v>345</v>
-      </c>
-      <c r="Y2" s="24" t="s">
-        <v>346</v>
-      </c>
-      <c r="Z2" s="24" t="s">
-        <v>347</v>
-      </c>
-      <c r="AA2" s="24" t="s">
-        <v>363</v>
-      </c>
-      <c r="AB2" s="24" t="s">
-        <v>343</v>
-      </c>
-      <c r="AC2" s="24" t="s">
-        <v>348</v>
-      </c>
-      <c r="AD2" s="24" t="s">
-        <v>350</v>
-      </c>
-      <c r="AE2" s="24" t="s">
-        <v>349</v>
-      </c>
-      <c r="AF2" s="24" t="s">
-        <v>364</v>
-      </c>
-      <c r="AG2" s="24" t="s">
-        <v>365</v>
-      </c>
-      <c r="AH2" s="24" t="s">
-        <v>366</v>
-      </c>
-      <c r="AI2" s="24" t="s">
-        <v>367</v>
-      </c>
-      <c r="AJ2" s="24" t="s">
-        <v>368</v>
-      </c>
-      <c r="AK2" s="24" t="s">
-        <v>369</v>
-      </c>
-      <c r="AL2" s="24" t="s">
-        <v>370</v>
-      </c>
-      <c r="AM2" s="24" t="s">
-        <v>371</v>
-      </c>
-      <c r="AN2" s="24" t="s">
-        <v>372</v>
-      </c>
-      <c r="AO2" s="24" t="s">
-        <v>373</v>
-      </c>
-      <c r="AP2" s="24" t="s">
-        <v>374</v>
-      </c>
-      <c r="AQ2" s="24" t="s">
-        <v>375</v>
-      </c>
-      <c r="AR2" s="24" t="s">
-        <v>355</v>
-      </c>
-      <c r="AS2" s="24" t="s">
-        <v>354</v>
-      </c>
-      <c r="AT2" s="24" t="s">
-        <v>376</v>
-      </c>
-      <c r="AU2" s="24" t="s">
-        <v>377</v>
-      </c>
-      <c r="AV2" s="24" t="s">
-        <v>378</v>
-      </c>
-      <c r="AW2" s="24" t="s">
-        <v>357</v>
-      </c>
-      <c r="AX2" s="24" t="s">
-        <v>379</v>
-      </c>
-      <c r="AY2" s="24" t="s">
-        <v>380</v>
-      </c>
-      <c r="AZ2" s="24" t="s">
-        <v>381</v>
-      </c>
-      <c r="BA2" s="24" t="s">
-        <v>382</v>
-      </c>
-      <c r="BB2" s="24" t="s">
-        <v>383</v>
-      </c>
-      <c r="BC2" s="24" t="s">
-        <v>358</v>
-      </c>
-      <c r="BD2" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="BE2" s="24" t="s">
-        <v>359</v>
-      </c>
-      <c r="BF2" s="24" t="s">
+      <c r="BN2" s="24" t="s">
+        <v>391</v>
+      </c>
+      <c r="BO2" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="BP2" s="24" t="s">
+        <v>393</v>
+      </c>
+      <c r="BQ2" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="BG2" s="24" t="s">
-        <v>393</v>
-      </c>
-      <c r="BH2" s="24" t="s">
+      <c r="BR2" s="24" t="s">
+        <v>395</v>
+      </c>
+      <c r="BS2" s="24" t="s">
         <v>396</v>
       </c>
-      <c r="BI2" s="24" t="s">
+      <c r="BT2" s="24" t="s">
         <v>397</v>
       </c>
-      <c r="BJ2" s="24" t="s">
+      <c r="BU2" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="BK2" s="24" t="s">
-        <v>415</v>
-      </c>
-      <c r="BL2" s="24" t="s">
-        <v>416</v>
-      </c>
-      <c r="BM2" s="24" t="s">
+      <c r="BV2" s="24" t="s">
         <v>399</v>
       </c>
-      <c r="BN2" s="24" t="s">
+      <c r="BW2" s="24" t="s">
         <v>400</v>
       </c>
-      <c r="BO2" s="24" t="s">
+      <c r="BX2" s="24" t="s">
         <v>401</v>
       </c>
-      <c r="BP2" s="24" t="s">
-        <v>402</v>
-      </c>
-      <c r="BQ2" s="24" t="s">
+      <c r="BY2" s="24" t="s">
+        <v>404</v>
+      </c>
+      <c r="BZ2" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="CA2" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="CB2" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="CC2" s="24" t="s">
         <v>403</v>
-      </c>
-      <c r="BR2" s="24" t="s">
-        <v>404</v>
-      </c>
-      <c r="BS2" s="24" t="s">
-        <v>405</v>
-      </c>
-      <c r="BT2" s="24" t="s">
-        <v>406</v>
-      </c>
-      <c r="BU2" s="24" t="s">
-        <v>407</v>
-      </c>
-      <c r="BV2" s="24" t="s">
-        <v>408</v>
-      </c>
-      <c r="BW2" s="24" t="s">
-        <v>409</v>
-      </c>
-      <c r="BX2" s="24" t="s">
-        <v>410</v>
-      </c>
-      <c r="BY2" s="24" t="s">
-        <v>413</v>
-      </c>
-      <c r="BZ2" s="24" t="s">
-        <v>414</v>
-      </c>
-      <c r="CA2" s="24" t="s">
-        <v>329</v>
-      </c>
-      <c r="CB2" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="CC2" s="24" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="3" spans="1:81" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>419</v>
-      </c>
+      <c r="B3" s="13"/>
       <c r="C3" s="13" t="s">
         <v>20</v>
       </c>
@@ -2382,10 +2401,10 @@
         <v>19</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>23</v>
@@ -2403,196 +2422,196 @@
         <v>1</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>26</v>
+        <v>417</v>
       </c>
       <c r="N3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="P3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="Q3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="R3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="S3" s="19" t="s">
         <v>31</v>
-      </c>
-      <c r="S3" s="19" t="s">
-        <v>32</v>
       </c>
       <c r="T3" s="13">
         <v>162</v>
       </c>
       <c r="U3" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="W3" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="X3" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="Y3" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="Z3" s="28" t="s">
+        <v>334</v>
+      </c>
+      <c r="AA3" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="AB3" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="AC3" s="28" t="s">
+        <v>343</v>
+      </c>
+      <c r="AD3" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="AE3" s="28" t="s">
+        <v>344</v>
+      </c>
+      <c r="AF3" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="AG3" s="26" t="s">
+        <v>428</v>
+      </c>
+      <c r="AH3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="V3" s="13" t="s">
+      <c r="AI3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="W3" s="27" t="s">
-        <v>340</v>
-      </c>
-      <c r="X3" s="27" t="s">
-        <v>341</v>
-      </c>
-      <c r="Y3" s="27" t="s">
-        <v>340</v>
-      </c>
-      <c r="Z3" s="28" t="s">
-        <v>342</v>
-      </c>
-      <c r="AA3" s="26" t="s">
+      <c r="AJ3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="AB3" s="27" t="s">
-        <v>340</v>
-      </c>
-      <c r="AC3" s="28" t="s">
-        <v>351</v>
-      </c>
-      <c r="AD3" s="27" t="s">
-        <v>340</v>
-      </c>
-      <c r="AE3" s="28" t="s">
+      <c r="AL3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN3" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="AO3" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="AP3" s="13" t="s">
+        <v>412</v>
+      </c>
+      <c r="AQ3" s="28" t="s">
+        <v>345</v>
+      </c>
+      <c r="AR3" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="AS3" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="AF3" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG3" s="26" t="s">
+      <c r="AT3" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="AH3" s="13" t="s">
+      <c r="AU3" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="AV3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="AI3" s="13" t="s">
+      <c r="AW3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="AJ3" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK3" s="13" t="s">
+      <c r="AX3" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AL3" s="13" t="s">
+      <c r="AY3" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AZ3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="BA3" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="BB3" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="BC3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AM3" s="13" t="s">
+      <c r="BD3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="BE3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AN3" s="13" t="s">
-        <v>420</v>
-      </c>
-      <c r="AO3" s="13" t="s">
-        <v>421</v>
-      </c>
-      <c r="AP3" s="13" t="s">
-        <v>422</v>
-      </c>
-      <c r="AQ3" s="28" t="s">
-        <v>353</v>
-      </c>
-      <c r="AR3" s="27" t="s">
-        <v>340</v>
-      </c>
-      <c r="AS3" s="28" t="s">
-        <v>360</v>
-      </c>
-      <c r="AT3" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AU3" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="AV3" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="AW3" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="AX3" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="AY3" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="AZ3" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="BA3" s="28" t="s">
-        <v>361</v>
-      </c>
-      <c r="BB3" s="28" t="s">
-        <v>362</v>
-      </c>
-      <c r="BC3" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="BD3" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="BE3" s="13" t="s">
-        <v>46</v>
-      </c>
       <c r="BF3" s="28" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="BG3" s="28" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="BH3" s="14" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="BI3" s="14" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="BJ3" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="BK3" s="30" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="BL3" s="14" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="BM3" s="14" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="BN3" s="13" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="BO3" s="13">
         <v>0</v>
       </c>
       <c r="BP3" s="13" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="BQ3" s="18" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="BR3" s="13" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="BS3" s="13" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="BT3" s="28" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="BU3" s="13" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="BV3" s="13">
         <v>20000</v>
       </c>
       <c r="BW3" s="13" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="BX3" s="13" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="BY3" s="13" t="b">
         <v>1</v>
@@ -2601,14 +2620,17 @@
         <v>1</v>
       </c>
       <c r="CA3" s="13" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="CB3" s="13" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="CC3" s="13" t="s">
-        <v>328</v>
-      </c>
+        <v>321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="N4" s="21"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2 B4:B1048576">
@@ -2639,13 +2661,7 @@
   <pageSetup orientation="portrait" r:id="rId4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8823927F-487D-4F54-8545-EB3D72C804CF}">
-          <x14:formula1>
-            <xm:f>MerchantCategoryDropDown!$A$2:$A$12</xm:f>
-          </x14:formula1>
-          <xm:sqref>U3</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{735B2064-5C67-4905-9284-FEA25FDEC912}">
           <x14:formula1>
             <xm:f>Merchant_TypeDropDown!$A$2:$A$215</xm:f>
@@ -2688,6 +2704,36 @@
           </x14:formula1>
           <xm:sqref>BS3</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AD4152DB-8622-48E0-893C-62A005DBA39D}">
+          <x14:formula1>
+            <xm:f>MerchantCategoryDropDown!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>M3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{770F3F41-2959-447D-BEE9-7855C0691ECB}">
+          <x14:formula1>
+            <xm:f>MerchantCategoryDropDown!$E$2:$E$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>P3 BJ3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FFD781CB-DE36-4599-B9D6-415875CB6036}">
+          <x14:formula1>
+            <xm:f>MerchantCategoryDropDown!$G$2:$G$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>L3 J3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EF556784-6FDE-4E69-A336-1616CADA3F19}">
+          <x14:formula1>
+            <xm:f>MerchantCategoryDropDown!$I$2:$I$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>V3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8823927F-487D-4F54-8545-EB3D72C804CF}">
+          <x14:formula1>
+            <xm:f>MerchantCategoryDropDown!$A$2:$A$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>U3</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -2705,32 +2751,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -2750,12 +2796,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.5703125" collapsed="true"/>
+    <col min="1" max="1" width="41.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -2765,32 +2811,32 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -2810,27 +2856,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="46.28515625" collapsed="true"/>
+    <col min="1" max="1" width="46.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -2843,16 +2889,16 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="67.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="1" max="1" width="67.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3048,84 +3094,145 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="3.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="3.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="3.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="3.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="3.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="3.7109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="3.7109375" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="3.7109375" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="3.7109375" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="3.7109375" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="3.7109375" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="3.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="G3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A12" xr:uid="{FD83EAB1-1DD5-4062-B109-C49590B4B40E}">
-      <formula1>$A$2:$A$12</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3135,1088 +3242,1088 @@
   <dimension ref="A1:A215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A205" sqref="A205"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="71.28515625" collapsed="true"/>
+    <col min="1" max="1" width="71.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="8" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="8" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="8" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="8" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="8" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="8" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="8" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="8" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="8" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="8" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="8" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="8" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="8" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="8" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="8" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="8" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="8" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="8" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="8" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="8" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="8" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="8" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="8" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="8" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="8" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="8" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="8" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="8" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="8" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="8" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="8" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="8" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="8" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="8" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="8" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="8" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="8" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="8" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="8" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="8" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="8" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="8" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="8" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="8" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="8" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="8" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="8" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="8" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="8" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="8" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="8" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="8" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="8" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="8" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="8" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="8" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="8" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" s="8" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="8" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="8" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="8" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="8" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="8" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -4234,12 +4341,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -4258,7 +4365,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="1" max="1" width="40.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -4268,127 +4375,127 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -4407,7 +4514,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="1" max="1" width="39.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -4417,37 +4524,37 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -4466,32 +4573,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="44.140625" collapsed="true"/>
+    <col min="1" max="1" width="44.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>